<commit_message>
FINAL check in, with full discussion and cleaner interval array structure.
</commit_message>
<xml_diff>
--- a/discussion/testLoad.xlsx
+++ b/discussion/testLoad.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="5450" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="5450" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="S50L1000 dup" sheetId="8" r:id="rId1"/>
@@ -3349,6 +3349,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3881,6 +3882,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3999,6 +4001,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4532,6 +4535,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4642,6 +4646,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5175,6 +5180,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5285,6 +5291,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5817,6 +5824,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5927,6 +5935,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6460,6 +6469,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15802,7 +15812,7 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView topLeftCell="A31" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
-      <selection activeCell="S41" sqref="S41"/>
+      <selection activeCell="Q41" sqref="Q41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18704,8 +18714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:G65"/>
+    <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>